<commit_message>
Cleanup Matlab code (it.1.1)
</commit_message>
<xml_diff>
--- a/matlab/Parameters/Par_HUN_2023-12-19_JN1.xlsx
+++ b/matlab/Parameters/Par_HUN_2023-12-19_JN1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -64,9 +64,6 @@
     <t xml:space="preserve">Pr_D</t>
   </si>
   <si>
-    <t xml:space="preserve">New_Cases_Shift</t>
-  </si>
-  <si>
     <t xml:space="preserve">beta0</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t xml:space="preserve">w_H</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Transient</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">Wild</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ez a táblázat már nem kompatibilis a fájl nevében megjelölt dátumnál régebbi kódokkal.</t>
   </si>
   <si>
     <t xml:space="preserve">Alpha</t>
@@ -171,7 +162,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -207,15 +198,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,12 +216,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF4000"/>
-        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -293,7 +271,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,10 +314,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -415,7 +389,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF4000"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -439,14 +413,14 @@
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.96"/>
@@ -461,11 +435,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="6.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="6.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,23 +496,19 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>43739</v>
@@ -575,31 +544,29 @@
         <v>0.205</v>
       </c>
       <c r="O2" s="5" t="n">
-        <v>12</v>
+        <v>0.33</v>
       </c>
       <c r="P2" s="5" t="n">
-        <v>0.33</v>
+        <v>1.5</v>
       </c>
       <c r="Q2" s="5" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" s="5"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="n">
@@ -636,36 +603,32 @@
         <v>0.205</v>
       </c>
       <c r="O3" s="8" t="n">
-        <v>12</v>
+        <v>0.33</v>
       </c>
       <c r="P3" s="8" t="n">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q3" s="8" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="S3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>23</v>
-      </c>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>44228</v>
@@ -701,34 +664,32 @@
         <v>0.26</v>
       </c>
       <c r="O4" s="8" t="n">
-        <v>12</v>
+        <v>0.5</v>
       </c>
       <c r="P4" s="8" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="Q4" s="8" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="R4" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="S4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="11"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="7" t="n">
         <v>44409</v>
@@ -764,34 +725,32 @@
         <v>0.24</v>
       </c>
       <c r="O5" s="8" t="n">
-        <v>10</v>
+        <v>0.83</v>
       </c>
       <c r="P5" s="8" t="n">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
       <c r="Q5" s="8" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="R5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="S5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="11"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="7" t="n">
         <v>44562</v>
@@ -827,33 +786,31 @@
         <v>0.18</v>
       </c>
       <c r="O6" s="8" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="P6" s="8" t="n">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="Q6" s="8" t="n">
-        <v>1.8</v>
+        <v>5</v>
       </c>
       <c r="R6" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="S6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF6" s="0"/>
+      <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="C7" s="12"/>
       <c r="D7" s="7" t="n">
         <v>44621</v>
       </c>
@@ -888,34 +845,32 @@
         <v>0.15</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="Q7" s="8" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="R7" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="S7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF7" s="0"/>
+      <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="7" t="n">
         <v>44727</v>
@@ -932,7 +887,7 @@
       <c r="H8" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="14" t="n">
+      <c r="I8" s="13" t="n">
         <v>5</v>
       </c>
       <c r="J8" s="8" t="n">
@@ -951,33 +906,31 @@
         <v>0.15</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="Q8" s="8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R8" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="S8" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T8" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF8" s="0"/>
+      <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="C9" s="12"/>
       <c r="D9" s="7" t="n">
         <v>44804</v>
       </c>
@@ -993,7 +946,7 @@
       <c r="H9" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="14" t="n">
+      <c r="I9" s="13" t="n">
         <v>6</v>
       </c>
       <c r="J9" s="8" t="n">
@@ -1012,34 +965,32 @@
         <v>0.15</v>
       </c>
       <c r="O9" s="8" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="P9" s="8" t="n">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R9" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="S9" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T9" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF9" s="0"/>
+      <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="D10" s="7" t="n">
         <v>44900</v>
@@ -1056,7 +1007,7 @@
       <c r="H10" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I10" s="14" t="n">
+      <c r="I10" s="13" t="n">
         <v>8</v>
       </c>
       <c r="J10" s="8" t="n">
@@ -1075,34 +1026,32 @@
         <v>0.15</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>1.9</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="8" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R10" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="S10" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T10" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF10" s="0"/>
+      <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>44962</v>
@@ -1119,7 +1068,7 @@
       <c r="H11" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="14" t="n">
+      <c r="I11" s="13" t="n">
         <v>10</v>
       </c>
       <c r="J11" s="8" t="n">
@@ -1138,34 +1087,32 @@
         <v>0.15</v>
       </c>
       <c r="O11" s="8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" s="8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="8" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R11" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="S11" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T11" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF11" s="0"/>
+      <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D12" s="7" t="n">
         <v>45153</v>
@@ -1182,7 +1129,7 @@
       <c r="H12" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I12" s="14" t="n">
+      <c r="I12" s="13" t="n">
         <v>10</v>
       </c>
       <c r="J12" s="8" t="n">
@@ -1201,34 +1148,32 @@
         <v>0.15</v>
       </c>
       <c r="O12" s="8" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="P12" s="8" t="n">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="Q12" s="8" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R12" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="S12" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T12" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF12" s="0"/>
+      <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D13" s="7" t="n">
         <v>45240</v>
@@ -1245,7 +1190,7 @@
       <c r="H13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="14" t="n">
+      <c r="I13" s="13" t="n">
         <v>10</v>
       </c>
       <c r="J13" s="8" t="n">
@@ -1264,34 +1209,32 @@
         <v>0.15</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="Q13" s="8" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R13" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="S13" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T13" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="AMF13" s="0"/>
+      <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="15" t="n">
+        <v>43</v>
+      </c>
+      <c r="D14" s="14" t="n">
         <v>46022</v>
       </c>
       <c r="E14" s="5" t="n">
@@ -1325,29 +1268,24 @@
         <v>0.15</v>
       </c>
       <c r="O14" s="5" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="P14" s="5" t="n">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="Q14" s="5" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R14" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="S14" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T14" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="AMF14" s="0"/>
+      <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="T3:T12"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>